<commit_message>
added the antennas that I'm buying
</commit_message>
<xml_diff>
--- a/hardware/radio_module/rev_a/radio_module_bom.xlsx
+++ b/hardware/radio_module/rev_a/radio_module_bom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="radio_module" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="286">
   <si>
     <t xml:space="preserve">Part</t>
   </si>
@@ -860,6 +860,24 @@
   </si>
   <si>
     <t xml:space="preserve">FH1600015CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSM Antenna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1050-1116-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lora Antenna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANT-868-CW-RH-SMA-ND</t>
   </si>
 </sst>
 </file>
@@ -869,11 +887,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -894,6 +913,14 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -938,12 +965,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -964,21 +995,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F103"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F103" activeCellId="0" sqref="F103"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B105" activeCellId="0" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.9030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="25.7448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.9642857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.719387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.6224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3002,7 +3033,33 @@
         <v>279</v>
       </c>
     </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F104" r:id="rId1" display="1050-1116-ND"/>
+    <hyperlink ref="F105" r:id="rId2" display="ANT-868-CW-RH-SMA-ND"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>